<commit_message>
XLSX daily template and convertion have been added...
</commit_message>
<xml_diff>
--- a/reports/operative_templ.xlsx
+++ b/reports/operative_templ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
@@ -217,6 +217,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF00000A"/>
       <name val="Liberation Serif;Times New Roman"/>
@@ -231,7 +232,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -246,6 +247,27 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -272,7 +294,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,8 +303,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -297,12 +319,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -313,11 +331,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,13 +426,17 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="20.9795918367347"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -479,230 +509,228 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="26.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="D11" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="10" t="n">
+      <c r="D12" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="10" t="n">
+      <c r="D13" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="10" t="n">
+      <c r="D14" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="12" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="n">
+      <c r="A15" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="10" t="n">
+      <c r="D15" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="12" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="10" t="n">
+      <c r="D16" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="10" t="n">
+      <c r="D17" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="12" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="6">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:F4"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.39375" right="0.39375" top="0.659027777777778" bottom="0.659027777777778" header="0.39375" footer="0.39375"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>

</xml_diff>

<commit_message>
New form operative templates for MREM is added... Reducer working in PointForm is fixed.
</commit_message>
<xml_diff>
--- a/reports/operative_templ.xlsx
+++ b/reports/operative_templ.xlsx
@@ -20,15 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
-  <si>
-    <t xml:space="preserve">Оперативный отчет</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Станция: {d[i].station}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        {d[i].values[i].date}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+  <si>
+    <t xml:space="preserve">Государственное казенное учреждение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Московской области</t>
+  </si>
+  <si>
+    <t xml:space="preserve">«Мособлэкомониторинг»</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лист  измерений концентраций вредных веществ в атмосферном воздухе №________</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Приложение к акту А/АВ   №_________ от ______________________________________)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Объект (наименование, координаты, адрес): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d[i].name} {d[i].lat}  { d[i].lon}    , {d[i].place}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Дата измерений: {d[i].date}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Результаты измерений:</t>
   </si>
   <si>
     <t xml:space="preserve">Параметры загрязнения</t>
@@ -49,7 +67,7 @@
     <t xml:space="preserve">дата</t>
   </si>
   <si>
-    <t xml:space="preserve">время</t>
+    <t xml:space="preserve">точное время завершения</t>
   </si>
   <si>
     <t xml:space="preserve">значение</t>
@@ -139,10 +157,19 @@
     <t xml:space="preserve">{d[i].values[i].Rain}</t>
   </si>
   <si>
-    <t xml:space="preserve">H пав., %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{d[i].values[i].Hin}</t>
+    <t xml:space="preserve">Примечание: результатом измерений является максимальная разовая концентрация.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Измерения проводил:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">должность  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  подпись     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">инициалы, фамилия</t>
   </si>
 </sst>
 </file>
@@ -152,7 +179,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -173,6 +200,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -183,6 +218,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF00000A"/>
       <name val="Liberation Serif;Times New Roman"/>
@@ -190,8 +232,29 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
@@ -204,7 +267,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -240,6 +303,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -266,7 +336,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,19 +345,43 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,7 +389,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,20 +397,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -396,22 +506,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.44"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,253 +532,433 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="17.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="7.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="7.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="B18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F19" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="26.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10" t="s">
+      <c r="B20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="D20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="23" customFormat="false" ht="26.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B28" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="n">
+      <c r="B29" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
+      <c r="B30" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+    </row>
+    <row r="36" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="E38" s="21"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="12">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:F18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.39375" right="0.39375" top="0.659027777777778" bottom="0.659027777777778" header="0.39375" footer="0.39375"/>

</xml_diff>